<commit_message>
asset/ truth_table control_unit rev2
</commit_message>
<xml_diff>
--- a/Control_Unit/assets/truth_table.xlsx
+++ b/Control_Unit/assets/truth_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrey\Documents\RISC-V\control_unit\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84804BD-45AF-4A7B-A0BD-D1FA77E3F819}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8911EAAE-51E9-41A4-9809-BBB0687F1907}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="915" yWindow="5355" windowWidth="21600" windowHeight="11385" xr2:uid="{C275EF26-4B58-43A6-85CE-BF07BF39F171}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C275EF26-4B58-43A6-85CE-BF07BF39F171}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>I/O</t>
   </si>
@@ -99,12 +99,6 @@
     <t>ALUOP1</t>
   </si>
   <si>
-    <t>ALUOP3</t>
-  </si>
-  <si>
-    <t>ALUOP2</t>
-  </si>
-  <si>
     <t>ALUOP0</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>New Hardware not in book</t>
+  </si>
+  <si>
+    <t>SD &amp; LD</t>
+  </si>
+  <si>
+    <t>ALU</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,6 +211,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,7 +537,7 @@
       <pane xSplit="5" ySplit="13" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,23 +568,23 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -619,7 +622,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -655,7 +658,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
@@ -691,7 +694,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -727,7 +730,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -763,7 +766,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -799,7 +802,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
@@ -835,7 +838,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -871,7 +874,7 @@
       <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
@@ -885,10 +888,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -905,7 +908,7 @@
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
@@ -939,7 +942,7 @@
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -973,7 +976,7 @@
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1007,7 +1010,7 @@
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1041,9 +1044,9 @@
       <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1074,77 +1077,120 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="A19" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>